<commit_message>
Added new Resources Links
</commit_message>
<xml_diff>
--- a/All Technologies Resources Links.xlsx
+++ b/All Technologies Resources Links.xlsx
@@ -1,41 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding-Notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Coding Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF5F777-A706-4682-A7EE-BD667B1D9836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" tabRatio="794" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="794" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Database" sheetId="5" r:id="rId1"/>
     <sheet name="JavaScript" sheetId="1" r:id="rId2"/>
     <sheet name="TypeScript" sheetId="2" r:id="rId3"/>
     <sheet name="React" sheetId="3" r:id="rId4"/>
-    <sheet name="Projects" sheetId="4" r:id="rId5"/>
+    <sheet name="Laravel" sheetId="6" r:id="rId5"/>
+    <sheet name="Notion" sheetId="7" r:id="rId6"/>
+    <sheet name="Projects" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="87">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -212,13 +208,98 @@
   </si>
   <si>
     <t>Leela Web Dev</t>
+  </si>
+  <si>
+    <t>Ajay Yadav</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=ACqpy4XFI14&amp;list=PLs20WIPqzFC4_HynK6wTRIKEqKHiZYpa4</t>
+  </si>
+  <si>
+    <t>Advanced Web Hindi</t>
+  </si>
+  <si>
+    <t>Laravel 8 Eloquent orm query builder tutorial</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=m0IsbkfONL4&amp;list=PL1TrjkMQ8UbVyIT0cDX-54gN5tunWZvaI</t>
+  </si>
+  <si>
+    <t>Laravel Eloquent Relationships</t>
+  </si>
+  <si>
+    <t>Qirolab</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=T-fV_T6IfDc&amp;t=792s</t>
+  </si>
+  <si>
+    <t>Code Agent</t>
+  </si>
+  <si>
+    <t>Complex CRUD Operations with Laravel</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=_LyEayVdqUM&amp;list=PLT51dtioU1pO7YgLOyNY0KF_3ny79D0BV</t>
+  </si>
+  <si>
+    <t>CodeHolic</t>
+  </si>
+  <si>
+    <t>Important YouTube Channels
+PHP, Laravel, Vue.js, etc.</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=4hBv0GwhyqM</t>
+  </si>
+  <si>
+    <t>Laravel ORM : Deep relationship, Fetch All Data In One Query</t>
+  </si>
+  <si>
+    <t>No. of Videos</t>
+  </si>
+  <si>
+    <t>How many Watched</t>
+  </si>
+  <si>
+    <t>Project Name</t>
+  </si>
+  <si>
+    <t>laravel_eloquent_relationships</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=C3xNJVtxZEs&amp;list=PLRB0wzP8AS_EQ6oXAjzH1qdpV4eVPd7Tp</t>
+  </si>
+  <si>
+    <t>Laravel 10 Ecommerce Project</t>
+  </si>
+  <si>
+    <t>PHP Tech Life</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=sccLfQ4_u10&amp;list=PLbGui_ZYuhijEqjCa63l0GkWh5EsG5iTR</t>
+  </si>
+  <si>
+    <t>Geeky Shows</t>
+  </si>
+  <si>
+    <t>Laravel Playlist</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/@creative_cove/videos</t>
+  </si>
+  <si>
+    <t>Creative Cove</t>
+  </si>
+  <si>
+    <t>All About Notion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,6 +318,13 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -277,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -302,6 +390,34 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -616,22 +732,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="118.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="118.88671875" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -645,7 +761,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -659,7 +775,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="36" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -673,7 +789,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -681,7 +797,7 @@
       <c r="C4" s="6"/>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -689,7 +805,7 @@
       <c r="C5" s="6"/>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -697,7 +813,7 @@
       <c r="C6" s="6"/>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -705,7 +821,7 @@
       <c r="C7" s="6"/>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -713,7 +829,7 @@
       <c r="C8" s="6"/>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -721,7 +837,7 @@
       <c r="C9" s="6"/>
       <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -729,7 +845,7 @@
       <c r="C10" s="6"/>
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -744,23 +860,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="128.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="28.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="128.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -774,7 +890,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -788,7 +904,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -802,7 +918,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -816,7 +932,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -830,7 +946,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -844,7 +960,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -858,7 +974,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -872,7 +988,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -886,7 +1002,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="36" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -900,7 +1016,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="36" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -914,7 +1030,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -928,7 +1044,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -938,7 +1054,7 @@
       <c r="C13" s="6"/>
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -955,22 +1071,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.88671875" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="115.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="115.109375" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -984,7 +1100,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -998,7 +1114,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1012,7 +1128,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1026,7 +1142,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1040,7 +1156,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1052,7 +1168,7 @@
       </c>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1070,22 +1186,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection sqref="A1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="118.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="118.88671875" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1099,7 +1215,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1113,7 +1229,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1125,7 +1241,7 @@
       </c>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1143,22 +1259,294 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{585CE38D-0378-4828-A164-46D58F9B0CE4}">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="58.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="17"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="18"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="18"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="18"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+    </row>
+    <row r="7" spans="1:7" ht="36" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="36" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" s="6">
+        <v>3</v>
+      </c>
+      <c r="F8" s="16">
+        <v>1</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="54" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>2</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:7" ht="36" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>3</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+    </row>
+    <row r="11" spans="1:7" ht="36" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>4</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+    </row>
+    <row r="12" spans="1:7" ht="36" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>5</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+    </row>
+    <row r="13" spans="1:7" ht="36" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>6</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+    </row>
+    <row r="14" spans="1:7" ht="36" x14ac:dyDescent="0.3">
+      <c r="A14" s="9">
+        <v>6</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D10" r:id="rId1" xr:uid="{B0437374-AB3D-4246-A389-12A75258A17A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58D452F7-8EDC-44D3-AFE3-99D814D5AD0A}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="118.88671875" style="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="15">
+        <v>1</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection sqref="A1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="118.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="118.88671875" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1172,7 +1560,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="54" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1186,7 +1574,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="36" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>

</xml_diff>